<commit_message>
updated script for autoconst viz file generation - looks like the file produced by this now sims in MDO code correctly. Had to fix problem with empty sunecl in calc_and_store_accesses
</commit_message>
<xml_diff>
--- a/parameters_gs_network.xlsx
+++ b/parameters_gs_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sim_parameters" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -167,9 +167,6 @@
     <t>KSAT</t>
   </si>
   <si>
-    <t>Piura, Dadaab, Darwin, Haleakala</t>
-  </si>
-  <si>
     <t>For optical</t>
   </si>
   <si>
@@ -351,6 +348,18 @@
   </si>
   <si>
     <t>Australia 9</t>
+  </si>
+  <si>
+    <t>Bridgesat</t>
+  </si>
+  <si>
+    <t>for LCRD mission</t>
+  </si>
+  <si>
+    <t>Equatorial</t>
+  </si>
+  <si>
+    <t>Equatorial alternative</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1118,7 @@
         <v>0.33420304699999998</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1129,7 +1138,7 @@
         <v>0.173694267573965</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1149,7 +1158,7 @@
         <v>0.34834365869822498</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1169,7 +1178,7 @@
         <v>0.57536225346745595</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1197,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1233,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1253,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1273,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1293,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1313,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1333,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1353,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1373,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1393,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16">
@@ -1445,19 +1454,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(G2,E2,H2,B2,I2,C2,J2)</f>
@@ -1475,19 +1484,19 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
         <v>48</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>51</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K22" si="0">CONCATENATE(G3,E3,H3,B3,I3,C3,J3)</f>
@@ -1505,19 +1514,19 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>50</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -1535,19 +1544,19 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>50</v>
-      </c>
-      <c r="J5" t="s">
-        <v>51</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -1565,19 +1574,19 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>50</v>
-      </c>
-      <c r="J6" t="s">
-        <v>51</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -1595,19 +1604,19 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>51</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -1625,19 +1634,19 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>49</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>50</v>
-      </c>
-      <c r="J8" t="s">
-        <v>51</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -1655,19 +1664,19 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>49</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>50</v>
-      </c>
-      <c r="J9" t="s">
-        <v>51</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -1685,19 +1694,19 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>49</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>50</v>
-      </c>
-      <c r="J10" t="s">
-        <v>51</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -1712,16 +1721,16 @@
       </c>
       <c r="E11" s="8"/>
       <c r="G11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
         <v>48</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>49</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>50</v>
-      </c>
-      <c r="J11" t="s">
-        <v>51</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -1736,16 +1745,16 @@
       </c>
       <c r="E12" s="8"/>
       <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
         <v>48</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>49</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>50</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -1760,16 +1769,16 @@
       </c>
       <c r="E13" s="8"/>
       <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
         <v>48</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>49</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>50</v>
-      </c>
-      <c r="J13" t="s">
-        <v>51</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -1784,16 +1793,16 @@
       </c>
       <c r="E14" s="8"/>
       <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
         <v>48</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>49</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>50</v>
-      </c>
-      <c r="J14" t="s">
-        <v>51</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -1808,16 +1817,16 @@
       </c>
       <c r="E15" s="8"/>
       <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
         <v>48</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>49</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>50</v>
-      </c>
-      <c r="J15" t="s">
-        <v>51</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -1832,16 +1841,16 @@
       </c>
       <c r="E16" s="8"/>
       <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>49</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>51</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -1856,16 +1865,16 @@
       </c>
       <c r="E17" s="8"/>
       <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
         <v>48</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>49</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>50</v>
-      </c>
-      <c r="J17" t="s">
-        <v>51</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -1880,16 +1889,16 @@
       </c>
       <c r="E18" s="8"/>
       <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
         <v>48</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>49</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>50</v>
-      </c>
-      <c r="J18" t="s">
-        <v>51</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
@@ -1904,16 +1913,16 @@
       </c>
       <c r="E19" s="8"/>
       <c r="G19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
         <v>48</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>49</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>50</v>
-      </c>
-      <c r="J19" t="s">
-        <v>51</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
@@ -1928,16 +1937,16 @@
       </c>
       <c r="E20" s="8"/>
       <c r="G20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" t="s">
         <v>48</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>49</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>50</v>
-      </c>
-      <c r="J20" t="s">
-        <v>51</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
@@ -1952,16 +1961,16 @@
       </c>
       <c r="E21" s="8"/>
       <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
         <v>48</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>49</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>50</v>
-      </c>
-      <c r="J21" t="s">
-        <v>51</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
@@ -1976,16 +1985,16 @@
       </c>
       <c r="E22" s="8"/>
       <c r="G22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
         <v>48</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>49</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>50</v>
-      </c>
-      <c r="J22" t="s">
-        <v>51</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
@@ -2267,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2298,7 +2307,7 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2309,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2320,7 +2329,7 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2328,10 +2337,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
-        <v>46</v>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2396,7 +2429,7 @@
         <v>0.33420304733727801</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2416,7 +2449,7 @@
         <v>0.71201602664496999</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2436,7 +2469,7 @@
         <v>0.42887760224852101</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2456,7 +2489,7 @@
         <v>0.65284443181656804</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2474,7 +2507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -2517,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2537,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2557,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2577,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2597,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2617,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2637,7 +2670,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2657,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2677,7 +2710,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2697,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2717,7 +2750,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2737,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2757,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2777,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2797,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2817,7 +2850,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2837,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16">
@@ -2921,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16">
@@ -2941,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16">
@@ -2961,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16">
@@ -2981,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16">
@@ -3001,7 +3034,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16">
@@ -3021,7 +3054,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16">
@@ -3041,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16">
@@ -3061,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16">
@@ -3081,7 +3114,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16">
@@ -3101,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16">
@@ -3121,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16">
@@ -3141,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16">
@@ -3161,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16">
@@ -3181,7 +3214,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16">
@@ -3201,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16">
@@ -3221,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16">
@@ -3241,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16">
@@ -3261,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16">
@@ -3281,7 +3314,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16">
@@ -3301,7 +3334,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3364,7 +3397,7 @@
         <v>0.33420304733727801</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3384,7 +3417,7 @@
         <v>0.173694267573965</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3404,7 +3437,7 @@
         <v>0.34834365869822498</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3424,7 +3457,7 @@
         <v>0.57536225346745595</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3488,7 +3521,7 @@
         <v>0.33420304733727801</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3508,7 +3541,7 @@
         <v>0.71201602664496999</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>